<commit_message>
upload figures and plots
new plots
</commit_message>
<xml_diff>
--- a/SLR/Full-Paper-Read/Data-Extraction.xlsx
+++ b/SLR/Full-Paper-Read/Data-Extraction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitto\Desktop\github\SECO-for-CPS-Development-Study\SLR\Full-Paper-Read\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66F9299-F792-4208-9C70-F944BAC10972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205379BA-8088-4692-B58D-785D2E4DEDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Extraction" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Challenges" sheetId="4" r:id="rId3"/>
     <sheet name="Challenges-Plots" sheetId="9" r:id="rId4"/>
     <sheet name="Challenges-Paper-Map" sheetId="10" r:id="rId5"/>
-    <sheet name="Methods" sheetId="5" r:id="rId6"/>
-    <sheet name="Application-Domain" sheetId="6" r:id="rId7"/>
-    <sheet name="Application-Domain-Plots" sheetId="8" r:id="rId8"/>
+    <sheet name="Chellenges-Links" sheetId="12" r:id="rId6"/>
+    <sheet name="Methods" sheetId="5" r:id="rId7"/>
+    <sheet name="Application-Domain" sheetId="6" r:id="rId8"/>
+    <sheet name="Application-Domain-Plots" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2807" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="505">
   <si>
     <t>Nr</t>
   </si>
@@ -1644,6 +1645,30 @@
   <si>
     <t>Tot. Challenges</t>
   </si>
+  <si>
+    <t>System Design and Architecture</t>
+  </si>
+  <si>
+    <t>Model-Based System Engineering</t>
+  </si>
+  <si>
+    <t>Quality Attributes</t>
+  </si>
+  <si>
+    <t>Longevity &amp; Maintainability</t>
+  </si>
+  <si>
+    <t>Development and Engineering Processes</t>
+  </si>
+  <si>
+    <t>Continuous System &amp; Software Engineering</t>
+  </si>
+  <si>
+    <t>Data and Interoperability</t>
+  </si>
+  <si>
+    <t>Stakeholder Engagement</t>
+  </si>
 </sst>
 </file>
 
@@ -1731,12 +1756,30 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -1881,7 +1924,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1941,6 +1984,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -3349,6 +3404,559 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.4009091802387689E-2"/>
+          <c:y val="0.12548417551902016"/>
+          <c:w val="0.50598036864652585"/>
+          <c:h val="0.72565349709254934"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Challenges-Plots'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Occurrence</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-5FBB-4B36-BACD-6036CAE3F478}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Challenges-Plots'!$F$2:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>Scalability</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reliability</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Longevity &amp; Manteinability</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Testing</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Adaptability</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Requirements Engineering</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Model-Based Systems Engineering</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Architecture</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Continuous Software &amp; System Engineering</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Stakeholder Engangement</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Interoperability</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Intelligence &amp; Automation</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Safety &amp; Security</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Challenges-Plots'!$G$2:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FADE-4F49-8518-FDE1E2A8E802}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="75"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.55332791805229686"/>
+          <c:y val="0.14114109314178364"/>
+          <c:w val="0.42997746274703352"/>
+          <c:h val="0.75944375358969196"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
@@ -3805,7 +4413,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -3856,9 +4464,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Application-Domain-Plots'!$G$2:$G$19</c:f>
+              <c:f>'Application-Domain-Plots'!$G$2:$G$18</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>Construction</c:v>
                 </c:pt>
@@ -3875,42 +4483,39 @@
                   <c:v>Medical and Health</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Others</c:v>
+                  <c:v>Railway</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Railway</c:v>
+                  <c:v>Avionics</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Avionics</c:v>
+                  <c:v>Cloud Computing</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Cloud Computing</c:v>
+                  <c:v>Aerospace</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Aerospace</c:v>
+                  <c:v>Telecommunication Systems</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Telecommunication Systems</c:v>
+                  <c:v>Smart Cities</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Smart Cities</c:v>
+                  <c:v>IoT</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>IoT</c:v>
+                  <c:v>Industry 4.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Industry 4.0</c:v>
+                  <c:v>Digital Life</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Digital Life</c:v>
+                  <c:v>Manufacturing</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Manufacturing</c:v>
+                  <c:v>Automotive</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Automotive</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>Application Domain Independent</c:v>
                 </c:pt>
               </c:strCache>
@@ -3918,10 +4523,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Application-Domain-Plots'!$H$2:$H$19</c:f>
+              <c:f>'Application-Domain-Plots'!$H$2:$H$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3944,10 +4549,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4</c:v>
@@ -3962,18 +4567,15 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
@@ -4291,6 +4893,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5337,6 +5979,525 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5839,7 +7000,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6454,6 +7615,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>174306</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30BA050E-4177-0C73-7D5E-5B14B3C0B7DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6461,16 +7658,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1464537</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>100829</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>242004</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>156550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>200297</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>177029</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>237922</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>42250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -36218,8 +37415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859FEB63-89FB-4D23-9EB9-9258A0939B83}">
   <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22:F27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36244,7 +37441,7 @@
       <c r="F1" s="32" t="s">
         <v>482</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="28" t="s">
         <v>471</v>
       </c>
     </row>
@@ -37746,8 +38943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A225FC7-5B91-49E9-90A8-BB1E2555E689}">
   <dimension ref="A1:AI173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41023,6 +42220,773 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447C371D-D69B-40D9-98CE-8524C96B5140}">
+  <dimension ref="A2:P16"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C2" s="39" t="s">
+        <v>491</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>490</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>485</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>494</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>500</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>484</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>489</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>502</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>488</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>398</v>
+      </c>
+      <c r="N2" s="39" t="s">
+        <v>409</v>
+      </c>
+      <c r="O2" s="39" t="s">
+        <v>483</v>
+      </c>
+      <c r="P2" s="39" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
+        <v>497</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>491</v>
+      </c>
+      <c r="C3" s="37">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="38"/>
+      <c r="B4" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="37">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="38"/>
+      <c r="B5" s="39" t="s">
+        <v>490</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="37">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
+        <v>499</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>485</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="37">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="38"/>
+      <c r="B7" s="39" t="s">
+        <v>494</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="37">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="38"/>
+      <c r="B8" s="39" t="s">
+        <v>500</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="37">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="38"/>
+      <c r="B9" s="39" t="s">
+        <v>484</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="37">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="38"/>
+      <c r="B10" s="39" t="s">
+        <v>489</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="37">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>501</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>502</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="37">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39" t="s">
+        <v>488</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="37">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="38" t="s">
+        <v>503</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>398</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="37">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39" t="s">
+        <v>409</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14" s="37">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="40" t="s">
+        <v>483</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>483</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+      <c r="O15" s="37">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="40" t="s">
+        <v>504</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>504</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16" s="37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -52795,7 +54759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -65008,12 +66972,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8D953F-A4C3-4367-A3C3-181C67FF2332}">
   <dimension ref="A1:H984"/>
   <sheetViews>
-    <sheetView topLeftCell="G6" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -65053,7 +67017,7 @@
         <v>462</v>
       </c>
       <c r="H2" s="27">
-        <f t="shared" ref="H2:H19" si="0">COUNTIF($B$2:$B$70,G2)</f>
+        <f t="shared" ref="H2:H6" si="0">COUNTIF($B$2:$B$70,G2)</f>
         <v>1</v>
       </c>
     </row>
@@ -65125,10 +67089,10 @@
         <v>446</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>406</v>
+        <v>456</v>
       </c>
       <c r="H7" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H7:H18" si="1">COUNTIF($B$2:$B$70,G7)</f>
         <v>2</v>
       </c>
     </row>
@@ -65140,10 +67104,10 @@
         <v>447</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>456</v>
+        <v>476</v>
       </c>
       <c r="H8" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -65155,11 +67119,11 @@
         <v>447</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H9" s="27">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -65170,11 +67134,11 @@
         <v>443</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>477</v>
+        <v>455</v>
       </c>
       <c r="H10" s="27">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -65185,10 +67149,10 @@
         <v>443</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>455</v>
+        <v>478</v>
       </c>
       <c r="H11" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -65200,10 +67164,10 @@
         <v>446</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="H12" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -65215,10 +67179,10 @@
         <v>451</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="H13" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -65230,10 +67194,10 @@
         <v>451</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H14" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -65245,11 +67209,11 @@
         <v>443</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>481</v>
+        <v>446</v>
       </c>
       <c r="H15" s="27">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -65260,10 +67224,10 @@
         <v>443</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="H16" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -65275,11 +67239,11 @@
         <v>446</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H17" s="27">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -65290,11 +67254,11 @@
         <v>443</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H18" s="27">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -65303,13 +67267,6 @@
       </c>
       <c r="B19" s="29" t="s">
         <v>443</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>443</v>
-      </c>
-      <c r="H19" s="27">
-        <f t="shared" si="0"/>
-        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>